<commit_message>
Add parameters for baseline numer of M, NK, T, and T_E
</commit_message>
<xml_diff>
--- a/par_IAV.xlsx
+++ b/par_IAV.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -93,6 +93,9 @@
   <si>
     <t>dM</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Baseline number</t>
   </si>
 </sst>
 </file>
@@ -227,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -257,6 +260,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2988,6 +2994,266 @@
         <a:xfrm>
           <a:off x="0" y="13449300"/>
           <a:ext cx="142875" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="图片 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="15392400"/>
+          <a:ext cx="209550" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="图片 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="16002000"/>
+          <a:ext cx="190500" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="图片 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="16211550"/>
+          <a:ext cx="161925" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="图片 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="16421100"/>
+          <a:ext cx="238125" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5942,10 +6208,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6425,6 +6691,66 @@
       </c>
       <c r="F31">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="48" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>10000</v>
+      </c>
+      <c r="E32">
+        <v>100000</v>
+      </c>
+      <c r="F32">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33">
+        <v>10000</v>
+      </c>
+      <c r="E33">
+        <v>100000</v>
+      </c>
+      <c r="F33">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34">
+        <v>10000</v>
+      </c>
+      <c r="E34">
+        <v>1000000</v>
+      </c>
+      <c r="F34">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35">
+        <v>100</v>
+      </c>
+      <c r="E35">
+        <v>10000</v>
+      </c>
+      <c r="F35">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Try in the assumption of clock disrupted
</commit_message>
<xml_diff>
--- a/par_IAV.xlsx
+++ b/par_IAV.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -231,7 +231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -261,6 +261,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -5623,8 +5626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" activeCellId="1" sqref="A29:XFD29 A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6053,7 +6056,7 @@
       <c r="B28" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="11"/>
       <c r="D28">
         <v>1E-4</v>
       </c>
@@ -6076,7 +6079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>

</xml_diff>